<commit_message>
qsort fixed, time averaging
</commit_message>
<xml_diff>
--- a/task3/task3_stats.xlsx
+++ b/task3/task3_stats.xlsx
@@ -2,20 +2,47 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="results_1" localSheetId="0">Лист1!$A$2:$C$20</definedName>
+    <definedName name="results_2" localSheetId="0">Лист1!$A$22:$C$62</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="results_1" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="866" sourceFile="C:\Users\asus\Documents\GitHub\A-DS\task3\results_1.txt" thousands=" " space="1" consecutive="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="results_2" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="866" sourceFile="C:\Users\asus\Documents\GitHub\A-DS\task3\results_2.txt" thousands=" " space="1" consecutive="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,7 +113,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -181,19 +208,19 @@
                   <c:v>35000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>45000</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>55000</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>65000</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>75000</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>85000</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>100000</c:v>
@@ -208,67 +235,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>5.0100000000000003E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.5625715255737299E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0044E-4</c:v>
+                  <c:v>1.56741142272949E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0044E-4</c:v>
+                  <c:v>2.40099430084228E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5016999999999999E-3</c:v>
+                  <c:v>1.15037202835083E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.4999999999999997E-3</c:v>
+                  <c:v>2.4154067039489701E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.1027000000000001E-2</c:v>
+                  <c:v>0.124992847442626</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.3539999999999999E-2</c:v>
+                  <c:v>0.22345049381256099</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.8565E-2</c:v>
+                  <c:v>0.31407842636108302</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.13759350000000001</c:v>
+                  <c:v>0.42658870220184297</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.19463250000000001</c:v>
+                  <c:v>0.50784227848052899</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.19262879999999999</c:v>
+                  <c:v>0.58597171306610096</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.24715999999999999</c:v>
+                  <c:v>0.65783522129058802</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.27467999999999998</c:v>
+                  <c:v>0.83109169006347605</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.33873999999999999</c:v>
+                  <c:v>0.90161526203155495</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.36724000000000001</c:v>
+                  <c:v>1.07037487030029</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.43744</c:v>
+                  <c:v>1.2641212224960301</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.50033000000000005</c:v>
+                  <c:v>1.3984990119934</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.62290999999999996</c:v>
+                  <c:v>1.7329136133193901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0650-4A23-B4F7-8ACE1B236369}"/>
             </c:ext>
@@ -326,19 +353,19 @@
                   <c:v>35000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>45000</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>55000</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>65000</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>75000</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>85000</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>100000</c:v>
@@ -359,61 +386,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>8.0003738403320299E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0044E-3</c:v>
+                  <c:v>1.9002437591552699E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.5043000000000002E-3</c:v>
+                  <c:v>1.4904570579528801E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2999999999999999E-2</c:v>
+                  <c:v>3.5953879356384201E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.10657</c:v>
+                  <c:v>0.27034285068511898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.22414000000000001</c:v>
+                  <c:v>0.61566247940063401</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.38024999999999998</c:v>
+                  <c:v>0.95005459785461399</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.54786000000000001</c:v>
+                  <c:v>1.41100511550903</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.79854000000000003</c:v>
+                  <c:v>1.8594833374023401</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.87560899999999997</c:v>
+                  <c:v>2.1532507181167602</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.08172</c:v>
+                  <c:v>2.7892245054244902</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.3934599999999999</c:v>
+                  <c:v>3.3736328124999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.6716800000000001</c:v>
+                  <c:v>4.4377735853195102</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.0723799999999999</c:v>
+                  <c:v>5.4838631629943801</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.5157600000000002</c:v>
+                  <c:v>6.9807576894760102</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.2871899999999998</c:v>
+                  <c:v>8.6270657777786202</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.85907</c:v>
+                  <c:v>11.183450603485101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0650-4A23-B4F7-8ACE1B236369}"/>
             </c:ext>
@@ -427,11 +454,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1498895296"/>
-        <c:axId val="1543215504"/>
+        <c:axId val="158918120"/>
+        <c:axId val="158918512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1498895296"/>
+        <c:axId val="158918120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100000"/>
@@ -513,15 +540,15 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1543215504"/>
+        <c:crossAx val="158918512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1543215504"/>
+        <c:axId val="158918512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4"/>
+          <c:max val="11.2"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -597,7 +624,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1498895296"/>
+        <c:crossAx val="158918120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -630,7 +657,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -722,28 +749,28 @@
                   <c:v>-0.45</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.39999999999999902</c:v>
+                  <c:v>-0.4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.34999999999999898</c:v>
+                  <c:v>-0.35</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.29999999999999899</c:v>
+                  <c:v>-0.3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.249999999999999</c:v>
+                  <c:v>-0.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.19999999999999901</c:v>
+                  <c:v>-0.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.149999999999999</c:v>
+                  <c:v>-0.15</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-9.9999999999999006E-2</c:v>
+                  <c:v>-0.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-4.9999999999998997E-2</c:v>
+                  <c:v>-0.05</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -818,133 +845,133 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>1.38792</c:v>
+                  <c:v>6.34441232681274E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2678400000000001</c:v>
+                  <c:v>6.4381422996520998E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2723500000000001</c:v>
+                  <c:v>6.3751063346862799E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2533300000000001</c:v>
+                  <c:v>6.4381747245788504E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1922900000000001</c:v>
+                  <c:v>6.4071550369262695E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.20231</c:v>
+                  <c:v>6.4066267013549796E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.36791</c:v>
+                  <c:v>6.4693951606750399E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1187499999999999</c:v>
+                  <c:v>6.6253852844238195E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.14978</c:v>
+                  <c:v>6.6563401222228993E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.01868</c:v>
+                  <c:v>6.7191438674926704E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0051699999999999</c:v>
+                  <c:v>7.2188830375671295E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.92962</c:v>
+                  <c:v>7.2507085800170901E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.82306999999999997</c:v>
+                  <c:v>7.2507214546203597E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.75549999999999995</c:v>
+                  <c:v>7.3130369186401298E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.68545999999999996</c:v>
+                  <c:v>7.0006833076476996E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.57088000000000005</c:v>
+                  <c:v>7.3126311302184999E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.50783999999999996</c:v>
+                  <c:v>7.5941309928894002E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.38325999999999999</c:v>
+                  <c:v>7.0629439353942794E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.28969</c:v>
+                  <c:v>7.3757963180541994E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.15060000000000001</c:v>
+                  <c:v>7.3757266998290993E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.1520000000000001E-2</c:v>
+                  <c:v>7.3444738388061495E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.15160000000000001</c:v>
+                  <c:v>7.34446907043457E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.26717999999999997</c:v>
+                  <c:v>7.2832369804382305E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.41428999999999999</c:v>
+                  <c:v>7.1253910064697196E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.51234000000000002</c:v>
+                  <c:v>7.5004405975341804E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.63292000000000004</c:v>
+                  <c:v>7.3443174362182603E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.67595000000000005</c:v>
+                  <c:v>7.1881828308105397E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.94762999999999997</c:v>
+                  <c:v>7.4069857597351005E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.86056999999999995</c:v>
+                  <c:v>7.2191686630248997E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.93613000000000002</c:v>
+                  <c:v>7.3132195472717196E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.99265999999999999</c:v>
+                  <c:v>6.8751077651977494E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.0306900000000001</c:v>
+                  <c:v>6.6256537437438895E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.1772899999999999</c:v>
+                  <c:v>6.6253819465637201E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.21933</c:v>
+                  <c:v>6.5003805160522399E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.2113100000000001</c:v>
+                  <c:v>6.4694709777831996E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.2028099999999999</c:v>
+                  <c:v>6.4381623268127394E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.22882</c:v>
+                  <c:v>6.4345264434814406E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.2403299999999999</c:v>
+                  <c:v>6.4376120567321699E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.42045</c:v>
+                  <c:v>6.51648426055908E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.32639</c:v>
+                  <c:v>6.4646196365356401E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.2763500000000001</c:v>
+                  <c:v>6.4378767013549804E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F0E2-40DF-B4BE-C05836CF3878}"/>
             </c:ext>
@@ -999,28 +1026,28 @@
                   <c:v>-0.45</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.39999999999999902</c:v>
+                  <c:v>-0.4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.34999999999999898</c:v>
+                  <c:v>-0.35</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.29999999999999899</c:v>
+                  <c:v>-0.3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.249999999999999</c:v>
+                  <c:v>-0.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.19999999999999901</c:v>
+                  <c:v>-0.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.149999999999999</c:v>
+                  <c:v>-0.15</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-9.9999999999999006E-2</c:v>
+                  <c:v>-0.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-4.9999999999998997E-2</c:v>
+                  <c:v>-0.05</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1095,133 +1122,133 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>4.052E-2</c:v>
+                  <c:v>0.12062912940979</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.3520000000000003E-2</c:v>
+                  <c:v>0.12063203334808301</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.1020000000000001E-2</c:v>
+                  <c:v>0.120944514274597</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.3529999999999999E-2</c:v>
+                  <c:v>0.121566624641418</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.2528999999999997E-2</c:v>
+                  <c:v>0.122189307212829</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.1029999999999997E-2</c:v>
+                  <c:v>0.122507166862487</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.4519999999999997E-2</c:v>
+                  <c:v>0.123754549026489</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.2029999999999998E-2</c:v>
+                  <c:v>0.124697775840759</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.3529999999999999E-2</c:v>
+                  <c:v>0.12719783306121801</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.2520000000000002E-2</c:v>
+                  <c:v>0.127507410049438</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.6030000000000001E-2</c:v>
+                  <c:v>0.12656988620758</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.453E-2</c:v>
+                  <c:v>0.129692201614379</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.403E-2</c:v>
+                  <c:v>0.13031977653503399</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.2040000000000003E-2</c:v>
+                  <c:v>0.13344149589538501</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.6030000000000001E-2</c:v>
+                  <c:v>0.134383096694946</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.5530000000000001E-2</c:v>
+                  <c:v>0.13219855308532699</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.9029999999999997E-2</c:v>
+                  <c:v>0.13969557762145901</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.0529999999999999E-2</c:v>
+                  <c:v>0.14031768798828101</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.9029999999999997E-2</c:v>
+                  <c:v>0.14125463485717701</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.0529999999999999E-2</c:v>
+                  <c:v>0.140339593887329</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.6530000000000002E-2</c:v>
+                  <c:v>0.140005240440368</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.8030000000000003E-2</c:v>
+                  <c:v>0.135632925033569</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.6530000000000002E-2</c:v>
+                  <c:v>0.13344917774200399</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.9529999999999998E-2</c:v>
+                  <c:v>0.13000685214996299</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.453E-2</c:v>
+                  <c:v>0.12875743865966699</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.2029999999999998E-2</c:v>
+                  <c:v>0.127190732955932</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.2529999999999998E-2</c:v>
+                  <c:v>0.123442039489746</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.0529999999999997E-2</c:v>
+                  <c:v>0.12000692844390801</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.9030000000000002E-2</c:v>
+                  <c:v>0.116878881454467</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.9030000000000002E-2</c:v>
+                  <c:v>0.114381651878356</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.8019999999999998E-2</c:v>
+                  <c:v>0.111881585121154</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.703E-2</c:v>
+                  <c:v>0.110319213867187</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.052E-2</c:v>
+                  <c:v>0.108131303787231</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.3020000000000003E-2</c:v>
+                  <c:v>0.106878328323364</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.8519999999999999E-2</c:v>
+                  <c:v>0.104065155982971</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.8519999999999999E-2</c:v>
+                  <c:v>0.10219322204589799</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.3520000000000001E-2</c:v>
+                  <c:v>0.103758716583251</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.4020000000000002E-2</c:v>
+                  <c:v>9.9695978164672794E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.5020000000000003E-2</c:v>
+                  <c:v>9.8127851486205994E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.252E-2</c:v>
+                  <c:v>9.8399901390075595E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.3020000000000001E-2</c:v>
+                  <c:v>9.8286700248718203E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F0E2-40DF-B4BE-C05836CF3878}"/>
             </c:ext>
@@ -1235,11 +1262,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1498895296"/>
-        <c:axId val="1543215504"/>
+        <c:axId val="158920080"/>
+        <c:axId val="158919296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1498895296"/>
+        <c:axId val="158920080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1322,15 +1349,16 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1543215504"/>
+        <c:crossAx val="158919296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1543215504"/>
+        <c:axId val="158919296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.4"/>
+          <c:max val="0.15000000000000002"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1405,7 +1433,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1498895296"/>
+        <c:crossAx val="158920080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1431,7 +1459,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75" l="0.25" r="0.25" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1441,16 +1469,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>904873</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1472,15 +1500,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1502,6 +1530,14 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results_2" growShrinkType="overwriteClear" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results_1" growShrinkType="overwriteClear" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1772,11 +1808,15 @@
   </sheetPr>
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.875" customWidth="1"/>
+    <col min="2" max="3" width="11.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1794,7 +1834,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>5.0100000000000003E-4</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1805,7 +1845,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1.5625715255737299E-3</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1816,10 +1856,10 @@
         <v>50</v>
       </c>
       <c r="B4">
-        <v>5.0044E-4</v>
+        <v>1.56741142272949E-3</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>8.0003738403320299E-4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1827,10 +1867,10 @@
         <v>100</v>
       </c>
       <c r="B5">
-        <v>5.0044E-4</v>
+        <v>2.40099430084228E-3</v>
       </c>
       <c r="C5">
-        <v>5.0044E-3</v>
+        <v>1.9002437591552699E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1838,10 +1878,10 @@
         <v>500</v>
       </c>
       <c r="B6">
-        <v>2.5016999999999999E-3</v>
+        <v>1.15037202835083E-2</v>
       </c>
       <c r="C6">
-        <v>5.5043000000000002E-3</v>
+        <v>1.4904570579528801E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1849,10 +1889,10 @@
         <v>1000</v>
       </c>
       <c r="B7">
-        <v>6.4999999999999997E-3</v>
+        <v>2.4154067039489701E-2</v>
       </c>
       <c r="C7">
-        <v>1.2999999999999999E-2</v>
+        <v>3.5953879356384201E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1860,10 +1900,10 @@
         <v>5000</v>
       </c>
       <c r="B8">
-        <v>4.1027000000000001E-2</v>
+        <v>0.124992847442626</v>
       </c>
       <c r="C8">
-        <v>0.10657</v>
+        <v>0.27034285068511898</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1871,10 +1911,10 @@
         <v>10000</v>
       </c>
       <c r="B9">
-        <v>6.3539999999999999E-2</v>
+        <v>0.22345049381256099</v>
       </c>
       <c r="C9">
-        <v>0.22414000000000001</v>
+        <v>0.61566247940063401</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1882,10 +1922,10 @@
         <v>15000</v>
       </c>
       <c r="B10">
-        <v>9.8565E-2</v>
+        <v>0.31407842636108302</v>
       </c>
       <c r="C10">
-        <v>0.38024999999999998</v>
+        <v>0.95005459785461399</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1893,10 +1933,10 @@
         <v>20000</v>
       </c>
       <c r="B11">
-        <v>0.13759350000000001</v>
+        <v>0.42658870220184297</v>
       </c>
       <c r="C11">
-        <v>0.54786000000000001</v>
+        <v>1.41100511550903</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1904,10 +1944,10 @@
         <v>25000</v>
       </c>
       <c r="B12">
-        <v>0.19463250000000001</v>
+        <v>0.50784227848052899</v>
       </c>
       <c r="C12">
-        <v>0.79854000000000003</v>
+        <v>1.8594833374023401</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1915,10 +1955,10 @@
         <v>30000</v>
       </c>
       <c r="B13">
-        <v>0.19262879999999999</v>
+        <v>0.58597171306610096</v>
       </c>
       <c r="C13">
-        <v>0.87560899999999997</v>
+        <v>2.1532507181167602</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1926,65 +1966,65 @@
         <v>35000</v>
       </c>
       <c r="B14">
-        <v>0.24715999999999999</v>
+        <v>0.65783522129058802</v>
       </c>
       <c r="C14">
-        <v>1.08172</v>
+        <v>2.7892245054244902</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>45000</v>
+        <v>40000</v>
       </c>
       <c r="B15">
-        <v>0.27467999999999998</v>
+        <v>0.83109169006347605</v>
       </c>
       <c r="C15">
-        <v>1.3934599999999999</v>
+        <v>3.3736328124999999</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="B16">
-        <v>0.33873999999999999</v>
+        <v>0.90161526203155495</v>
       </c>
       <c r="C16">
-        <v>1.6716800000000001</v>
+        <v>4.4377735853195102</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>65000</v>
+        <v>60000</v>
       </c>
       <c r="B17">
-        <v>0.36724000000000001</v>
+        <v>1.07037487030029</v>
       </c>
       <c r="C17">
-        <v>2.0723799999999999</v>
+        <v>5.4838631629943801</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>75000</v>
+        <v>70000</v>
       </c>
       <c r="B18">
-        <v>0.43744</v>
+        <v>1.2641212224960301</v>
       </c>
       <c r="C18">
-        <v>2.5157600000000002</v>
+        <v>6.9807576894760102</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>85000</v>
+        <v>80000</v>
       </c>
       <c r="B19">
-        <v>0.50033000000000005</v>
+        <v>1.3984990119934</v>
       </c>
       <c r="C19">
-        <v>3.2871899999999998</v>
+        <v>8.6270657777786202</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1992,10 +2032,10 @@
         <v>100000</v>
       </c>
       <c r="B20">
-        <v>0.62290999999999996</v>
+        <v>1.7329136133193901</v>
       </c>
       <c r="C20">
-        <v>3.85907</v>
+        <v>11.183450603485101</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2014,10 +2054,10 @@
         <v>-1</v>
       </c>
       <c r="B22">
-        <v>1.38792</v>
+        <v>6.34441232681274E-2</v>
       </c>
       <c r="C22">
-        <v>4.052E-2</v>
+        <v>0.12062912940979</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2025,10 +2065,10 @@
         <v>-0.95</v>
       </c>
       <c r="B23">
-        <v>1.2678400000000001</v>
+        <v>6.4381422996520998E-2</v>
       </c>
       <c r="C23">
-        <v>4.3520000000000003E-2</v>
+        <v>0.12063203334808301</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2036,10 +2076,10 @@
         <v>-0.9</v>
       </c>
       <c r="B24">
-        <v>1.2723500000000001</v>
+        <v>6.3751063346862799E-2</v>
       </c>
       <c r="C24">
-        <v>4.1020000000000001E-2</v>
+        <v>0.120944514274597</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2047,10 +2087,10 @@
         <v>-0.85</v>
       </c>
       <c r="B25">
-        <v>1.2533300000000001</v>
+        <v>6.4381747245788504E-2</v>
       </c>
       <c r="C25">
-        <v>4.3529999999999999E-2</v>
+        <v>0.121566624641418</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2058,10 +2098,10 @@
         <v>-0.8</v>
       </c>
       <c r="B26">
-        <v>1.1922900000000001</v>
+        <v>6.4071550369262695E-2</v>
       </c>
       <c r="C26">
-        <v>4.2528999999999997E-2</v>
+        <v>0.122189307212829</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2069,10 +2109,10 @@
         <v>-0.75</v>
       </c>
       <c r="B27">
-        <v>1.20231</v>
+        <v>6.4066267013549796E-2</v>
       </c>
       <c r="C27">
-        <v>4.1029999999999997E-2</v>
+        <v>0.122507166862487</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2080,10 +2120,10 @@
         <v>-0.7</v>
       </c>
       <c r="B28">
-        <v>1.36791</v>
+        <v>6.4693951606750399E-2</v>
       </c>
       <c r="C28">
-        <v>4.4519999999999997E-2</v>
+        <v>0.123754549026489</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2091,10 +2131,10 @@
         <v>-0.65</v>
       </c>
       <c r="B29">
-        <v>1.1187499999999999</v>
+        <v>6.6253852844238195E-2</v>
       </c>
       <c r="C29">
-        <v>4.2029999999999998E-2</v>
+        <v>0.124697775840759</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2102,10 +2142,10 @@
         <v>-0.6</v>
       </c>
       <c r="B30">
-        <v>1.14978</v>
+        <v>6.6563401222228993E-2</v>
       </c>
       <c r="C30">
-        <v>4.3529999999999999E-2</v>
+        <v>0.12719783306121801</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2113,10 +2153,10 @@
         <v>-0.55000000000000004</v>
       </c>
       <c r="B31">
-        <v>1.01868</v>
+        <v>6.7191438674926704E-2</v>
       </c>
       <c r="C31">
-        <v>4.2520000000000002E-2</v>
+        <v>0.127507410049438</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2124,10 +2164,10 @@
         <v>-0.5</v>
       </c>
       <c r="B32">
-        <v>1.0051699999999999</v>
+        <v>7.2188830375671295E-2</v>
       </c>
       <c r="C32">
-        <v>4.6030000000000001E-2</v>
+        <v>0.12656988620758</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2135,98 +2175,98 @@
         <v>-0.45</v>
       </c>
       <c r="B33">
-        <v>0.92962</v>
+        <v>7.2507085800170901E-2</v>
       </c>
       <c r="C33">
-        <v>4.453E-2</v>
+        <v>0.129692201614379</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>-0.39999999999999902</v>
+        <v>-0.4</v>
       </c>
       <c r="B34">
-        <v>0.82306999999999997</v>
+        <v>7.2507214546203597E-2</v>
       </c>
       <c r="C34">
-        <v>4.403E-2</v>
+        <v>0.13031977653503399</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>-0.34999999999999898</v>
+        <v>-0.35</v>
       </c>
       <c r="B35">
-        <v>0.75549999999999995</v>
+        <v>7.3130369186401298E-2</v>
       </c>
       <c r="C35">
-        <v>5.2040000000000003E-2</v>
+        <v>0.13344149589538501</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>-0.29999999999999899</v>
+        <v>-0.3</v>
       </c>
       <c r="B36">
-        <v>0.68545999999999996</v>
+        <v>7.0006833076476996E-2</v>
       </c>
       <c r="C36">
-        <v>4.6030000000000001E-2</v>
+        <v>0.134383096694946</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>-0.249999999999999</v>
+        <v>-0.25</v>
       </c>
       <c r="B37">
-        <v>0.57088000000000005</v>
+        <v>7.3126311302184999E-2</v>
       </c>
       <c r="C37">
-        <v>4.5530000000000001E-2</v>
+        <v>0.13219855308532699</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>-0.19999999999999901</v>
+        <v>-0.2</v>
       </c>
       <c r="B38">
-        <v>0.50783999999999996</v>
+        <v>7.5941309928894002E-2</v>
       </c>
       <c r="C38">
-        <v>4.9029999999999997E-2</v>
+        <v>0.13969557762145901</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>-0.149999999999999</v>
+        <v>-0.15</v>
       </c>
       <c r="B39">
-        <v>0.38325999999999999</v>
+        <v>7.0629439353942794E-2</v>
       </c>
       <c r="C39">
-        <v>5.0529999999999999E-2</v>
+        <v>0.14031768798828101</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>-9.9999999999999006E-2</v>
+        <v>-0.1</v>
       </c>
       <c r="B40">
-        <v>0.28969</v>
+        <v>7.3757963180541994E-2</v>
       </c>
       <c r="C40">
-        <v>4.9029999999999997E-2</v>
+        <v>0.14125463485717701</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>-4.9999999999998997E-2</v>
+        <v>-0.05</v>
       </c>
       <c r="B41">
-        <v>0.15060000000000001</v>
+        <v>7.3757266998290993E-2</v>
       </c>
       <c r="C41">
-        <v>5.0529999999999999E-2</v>
+        <v>0.140339593887329</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2234,10 +2274,10 @@
         <v>0</v>
       </c>
       <c r="B42">
-        <v>2.1520000000000001E-2</v>
+        <v>7.3444738388061495E-2</v>
       </c>
       <c r="C42">
-        <v>4.6530000000000002E-2</v>
+        <v>0.140005240440368</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -2245,10 +2285,10 @@
         <v>0.05</v>
       </c>
       <c r="B43">
-        <v>0.15160000000000001</v>
+        <v>7.34446907043457E-2</v>
       </c>
       <c r="C43">
-        <v>4.8030000000000003E-2</v>
+        <v>0.135632925033569</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2256,10 +2296,10 @@
         <v>0.1</v>
       </c>
       <c r="B44">
-        <v>0.26717999999999997</v>
+        <v>7.2832369804382305E-2</v>
       </c>
       <c r="C44">
-        <v>4.6530000000000002E-2</v>
+        <v>0.13344917774200399</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2267,10 +2307,10 @@
         <v>0.15</v>
       </c>
       <c r="B45">
-        <v>0.41428999999999999</v>
+        <v>7.1253910064697196E-2</v>
       </c>
       <c r="C45">
-        <v>4.9529999999999998E-2</v>
+        <v>0.13000685214996299</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2278,10 +2318,10 @@
         <v>0.2</v>
       </c>
       <c r="B46">
-        <v>0.51234000000000002</v>
+        <v>7.5004405975341804E-2</v>
       </c>
       <c r="C46">
-        <v>4.453E-2</v>
+        <v>0.12875743865966699</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2289,10 +2329,10 @@
         <v>0.25</v>
       </c>
       <c r="B47">
-        <v>0.63292000000000004</v>
+        <v>7.3443174362182603E-2</v>
       </c>
       <c r="C47">
-        <v>4.2029999999999998E-2</v>
+        <v>0.127190732955932</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2300,10 +2340,10 @@
         <v>0.3</v>
       </c>
       <c r="B48">
-        <v>0.67595000000000005</v>
+        <v>7.1881828308105397E-2</v>
       </c>
       <c r="C48">
-        <v>4.2529999999999998E-2</v>
+        <v>0.123442039489746</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2311,10 +2351,10 @@
         <v>0.35</v>
       </c>
       <c r="B49">
-        <v>0.94762999999999997</v>
+        <v>7.4069857597351005E-2</v>
       </c>
       <c r="C49">
-        <v>4.0529999999999997E-2</v>
+        <v>0.12000692844390801</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2322,10 +2362,10 @@
         <v>0.4</v>
       </c>
       <c r="B50">
-        <v>0.86056999999999995</v>
+        <v>7.2191686630248997E-2</v>
       </c>
       <c r="C50">
-        <v>3.9030000000000002E-2</v>
+        <v>0.116878881454467</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2333,10 +2373,10 @@
         <v>0.45</v>
       </c>
       <c r="B51">
-        <v>0.93613000000000002</v>
+        <v>7.3132195472717196E-2</v>
       </c>
       <c r="C51">
-        <v>3.9030000000000002E-2</v>
+        <v>0.114381651878356</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -2344,10 +2384,10 @@
         <v>0.5</v>
       </c>
       <c r="B52">
-        <v>0.99265999999999999</v>
+        <v>6.8751077651977494E-2</v>
       </c>
       <c r="C52">
-        <v>3.8019999999999998E-2</v>
+        <v>0.111881585121154</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2355,10 +2395,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="B53">
-        <v>1.0306900000000001</v>
+        <v>6.6256537437438895E-2</v>
       </c>
       <c r="C53">
-        <v>3.703E-2</v>
+        <v>0.110319213867187</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -2366,10 +2406,10 @@
         <v>0.6</v>
       </c>
       <c r="B54">
-        <v>1.1772899999999999</v>
+        <v>6.6253819465637201E-2</v>
       </c>
       <c r="C54">
-        <v>4.052E-2</v>
+        <v>0.108131303787231</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2377,10 +2417,10 @@
         <v>0.65</v>
       </c>
       <c r="B55">
-        <v>1.21933</v>
+        <v>6.5003805160522399E-2</v>
       </c>
       <c r="C55">
-        <v>4.3020000000000003E-2</v>
+        <v>0.106878328323364</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -2388,10 +2428,10 @@
         <v>0.7</v>
       </c>
       <c r="B56">
-        <v>1.2113100000000001</v>
+        <v>6.4694709777831996E-2</v>
       </c>
       <c r="C56">
-        <v>3.8519999999999999E-2</v>
+        <v>0.104065155982971</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -2399,10 +2439,10 @@
         <v>0.75</v>
       </c>
       <c r="B57">
-        <v>1.2028099999999999</v>
+        <v>6.4381623268127394E-2</v>
       </c>
       <c r="C57">
-        <v>3.8519999999999999E-2</v>
+        <v>0.10219322204589799</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -2410,10 +2450,10 @@
         <v>0.8</v>
       </c>
       <c r="B58">
-        <v>1.22882</v>
+        <v>6.4345264434814406E-2</v>
       </c>
       <c r="C58">
-        <v>3.3520000000000001E-2</v>
+        <v>0.103758716583251</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2421,10 +2461,10 @@
         <v>0.85</v>
       </c>
       <c r="B59">
-        <v>1.2403299999999999</v>
+        <v>6.4376120567321699E-2</v>
       </c>
       <c r="C59">
-        <v>3.4020000000000002E-2</v>
+        <v>9.9695978164672794E-2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2432,10 +2472,10 @@
         <v>0.9</v>
       </c>
       <c r="B60">
-        <v>1.42045</v>
+        <v>6.51648426055908E-2</v>
       </c>
       <c r="C60">
-        <v>3.5020000000000003E-2</v>
+        <v>9.8127851486205994E-2</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -2443,10 +2483,10 @@
         <v>0.95</v>
       </c>
       <c r="B61">
-        <v>1.32639</v>
+        <v>6.4646196365356401E-2</v>
       </c>
       <c r="C61">
-        <v>3.252E-2</v>
+        <v>9.8399901390075595E-2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -2454,15 +2494,15 @@
         <v>1</v>
       </c>
       <c r="B62">
-        <v>1.2763500000000001</v>
+        <v>6.4378767013549804E-2</v>
       </c>
       <c r="C62">
-        <v>3.3020000000000001E-2</v>
+        <v>9.8286700248718203E-2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="88" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="67" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>